<commit_message>
I think this is the final
</commit_message>
<xml_diff>
--- a/src/Analysis/fitting_results.xlsx
+++ b/src/Analysis/fitting_results.xlsx
@@ -429,7 +429,7 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -469,11 +469,11 @@
         <v>29955.034578565901</v>
       </c>
       <c r="G2">
-        <f t="shared" ref="G2:G10" si="1">F2-F$12</f>
+        <f t="shared" ref="G2:G9" si="1">F2-F$12</f>
         <v>0</v>
       </c>
       <c r="H2">
-        <f t="shared" ref="H2:H10" si="2">G2/40</f>
+        <f t="shared" ref="H2:H9" si="2">G2/40</f>
         <v>0</v>
       </c>
     </row>
@@ -643,22 +643,22 @@
         <v>13</v>
       </c>
       <c r="C10">
-        <v>11696</v>
+        <v>10300.4335332544</v>
       </c>
       <c r="D10">
-        <v>21305</v>
+        <v>20071.046480664001</v>
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
-        <v>33001</v>
+        <v>30371.480013918401</v>
       </c>
       <c r="G10">
         <f>F10-F$12</f>
-        <v>3045.965421434099</v>
+        <v>416.44543535249977</v>
       </c>
       <c r="H10">
         <f>G10/40</f>
-        <v>76.14913553585248</v>
+        <v>10.411135883812495</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>